<commit_message>
Updated results script with imputed case models and added some simple visual sensitivity plots to see whether there was a visible difference between transformed or converted effect sizes and sampling variances
</commit_message>
<xml_diff>
--- a/Analysis/Comp_all_plant.xlsx
+++ b/Analysis/Comp_all_plant.xlsx
@@ -568,6 +568,11 @@
       <c r="T2">
         <v>5.059644256269408</v>
       </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V2" t="inlineStr">
         <is>
           <t>N</t>
@@ -659,6 +664,11 @@
       <c r="T3">
         <v>5.059644256269408</v>
       </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V3" t="inlineStr">
         <is>
           <t>N</t>
@@ -750,6 +760,11 @@
       <c r="T4">
         <v>4.743416490252569</v>
       </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V4" t="inlineStr">
         <is>
           <t>N</t>
@@ -841,6 +856,11 @@
       <c r="T5">
         <v>4.427188724235731</v>
       </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V5" t="inlineStr">
         <is>
           <t>N</t>
@@ -932,6 +952,11 @@
       <c r="T6">
         <v>4.427188724235731</v>
       </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V6" t="inlineStr">
         <is>
           <t>N</t>
@@ -1023,6 +1048,11 @@
       <c r="T7">
         <v>3.794733192202055</v>
       </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V7" t="inlineStr">
         <is>
           <t>N</t>
@@ -1114,6 +1144,11 @@
       <c r="T8">
         <v>3.794733192202055</v>
       </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V8" t="inlineStr">
         <is>
           <t>N</t>
@@ -1205,6 +1240,11 @@
       <c r="T9">
         <v>3.441099864697506</v>
       </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V9" t="inlineStr">
         <is>
           <t>N</t>
@@ -1296,6 +1336,11 @@
       <c r="T10">
         <v>3.441099864697503</v>
       </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V10" t="inlineStr">
         <is>
           <t>N</t>
@@ -1387,6 +1432,11 @@
       <c r="T11">
         <v>2.402277264034108</v>
       </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V11" t="inlineStr">
         <is>
           <t>N</t>
@@ -1478,6 +1528,11 @@
       <c r="T12">
         <v>1.882865963702409</v>
       </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V12" t="inlineStr">
         <is>
           <t>N</t>
@@ -1566,6 +1621,11 @@
       <c r="T13">
         <v>13.92</v>
       </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V13" t="inlineStr">
         <is>
           <t>N</t>
@@ -1654,6 +1714,11 @@
       <c r="T14">
         <v>2.74</v>
       </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V14" t="inlineStr">
         <is>
           <t>N</t>
@@ -1742,6 +1807,11 @@
       <c r="T15">
         <v>3.34</v>
       </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V15" t="inlineStr">
         <is>
           <t>N</t>
@@ -1830,6 +1900,11 @@
       <c r="T16">
         <v>8.34</v>
       </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V16" t="inlineStr">
         <is>
           <t>N</t>
@@ -1918,6 +1993,11 @@
       <c r="T17">
         <v>5.17</v>
       </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V17" t="inlineStr">
         <is>
           <t>N</t>
@@ -2006,6 +2086,11 @@
       <c r="T18">
         <v>4.38</v>
       </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V18" t="inlineStr">
         <is>
           <t>N</t>
@@ -2097,6 +2182,11 @@
       <c r="T19">
         <v>0.894427190999916</v>
       </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V19" t="inlineStr">
         <is>
           <t>N</t>
@@ -2188,6 +2278,11 @@
       <c r="T20">
         <v>0.894427190999916</v>
       </c>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V20" t="inlineStr">
         <is>
           <t>N</t>
@@ -2279,6 +2374,11 @@
       <c r="T21">
         <v>0.894427190999916</v>
       </c>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V21" t="inlineStr">
         <is>
           <t>N</t>
@@ -2370,6 +2470,11 @@
       <c r="T22">
         <v>0.894427190999916</v>
       </c>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V22" t="inlineStr">
         <is>
           <t>N</t>
@@ -2461,6 +2566,11 @@
       <c r="T23">
         <v>0.894427190999916</v>
       </c>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V23" t="inlineStr">
         <is>
           <t>N</t>
@@ -2552,6 +2662,11 @@
       <c r="T24">
         <v>4.47213595499958</v>
       </c>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V24" t="inlineStr">
         <is>
           <t>N</t>
@@ -2643,6 +2758,11 @@
       <c r="T25">
         <v>4.47213595499958</v>
       </c>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V25" t="inlineStr">
         <is>
           <t>N</t>
@@ -2734,6 +2854,11 @@
       <c r="T26">
         <v>4.47213595499958</v>
       </c>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V26" t="inlineStr">
         <is>
           <t>N</t>
@@ -2825,6 +2950,11 @@
       <c r="T27">
         <v>4.47213595499958</v>
       </c>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V27" t="inlineStr">
         <is>
           <t>N</t>
@@ -2916,6 +3046,11 @@
       <c r="T28">
         <v>4.47213595499958</v>
       </c>
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V28" t="inlineStr">
         <is>
           <t>N</t>
@@ -3007,6 +3142,11 @@
       <c r="T29">
         <v>4.024922359499622</v>
       </c>
+      <c r="U29" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V29" t="inlineStr">
         <is>
           <t>N</t>
@@ -3098,6 +3238,11 @@
       <c r="T30">
         <v>4.024922359499622</v>
       </c>
+      <c r="U30" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V30" t="inlineStr">
         <is>
           <t>N</t>
@@ -3189,6 +3334,11 @@
       <c r="T31">
         <v>4.024922359499622</v>
       </c>
+      <c r="U31" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V31" t="inlineStr">
         <is>
           <t>N</t>
@@ -3280,6 +3430,11 @@
       <c r="T32">
         <v>4.024922359499622</v>
       </c>
+      <c r="U32" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V32" t="inlineStr">
         <is>
           <t>N</t>
@@ -3371,6 +3526,11 @@
       <c r="T33">
         <v>4.024922359499622</v>
       </c>
+      <c r="U33" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V33" t="inlineStr">
         <is>
           <t>N</t>
@@ -3462,6 +3622,11 @@
       <c r="T34">
         <v>10.00502963814729</v>
       </c>
+      <c r="U34" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V34" t="inlineStr">
         <is>
           <t>N</t>
@@ -3553,6 +3718,11 @@
       <c r="T35">
         <v>10.00502963814729</v>
       </c>
+      <c r="U35" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V35" t="inlineStr">
         <is>
           <t>N</t>
@@ -3644,6 +3814,11 @@
       <c r="T36">
         <v>6.261851822108053</v>
       </c>
+      <c r="U36" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V36" t="inlineStr">
         <is>
           <t>N</t>
@@ -3735,6 +3910,11 @@
       <c r="T37">
         <v>1.43927095402817</v>
       </c>
+      <c r="U37" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V37" t="inlineStr">
         <is>
           <t>N</t>
@@ -3826,6 +4006,11 @@
       <c r="T38">
         <v>0.9595139693521195</v>
       </c>
+      <c r="U38" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V38" t="inlineStr">
         <is>
           <t>N</t>
@@ -3917,6 +4102,11 @@
       <c r="T39">
         <v>0.9595139693521195</v>
       </c>
+      <c r="U39" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V39" t="inlineStr">
         <is>
           <t>N</t>
@@ -4008,6 +4198,11 @@
       <c r="T40">
         <v>9.642059692022496</v>
       </c>
+      <c r="U40" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V40" t="inlineStr">
         <is>
           <t>N</t>
@@ -4099,6 +4294,11 @@
       <c r="T41">
         <v>8.570719726242247</v>
       </c>
+      <c r="U41" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V41" t="inlineStr">
         <is>
           <t>N</t>
@@ -4190,6 +4390,11 @@
       <c r="T42">
         <v>8.570719726242247</v>
       </c>
+      <c r="U42" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V42" t="inlineStr">
         <is>
           <t>N</t>
@@ -4281,6 +4486,11 @@
       <c r="T43">
         <v>54.77225575051661</v>
       </c>
+      <c r="U43" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V43" t="inlineStr">
         <is>
           <t>N</t>
@@ -4372,6 +4582,11 @@
       <c r="T44">
         <v>48.32846095633845</v>
       </c>
+      <c r="U44" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V44" t="inlineStr">
         <is>
           <t>N</t>
@@ -4463,6 +4678,11 @@
       <c r="T45">
         <v>48.32846095633845</v>
       </c>
+      <c r="U45" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V45" t="inlineStr">
         <is>
           <t>N</t>
@@ -7518,6 +7738,11 @@
       <c r="R77">
         <v>20</v>
       </c>
+      <c r="U77" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V77" t="inlineStr">
         <is>
           <t>N</t>
@@ -7603,6 +7828,11 @@
       <c r="R78">
         <v>20</v>
       </c>
+      <c r="U78" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V78" t="inlineStr">
         <is>
           <t>N</t>
@@ -7688,6 +7918,11 @@
       <c r="R79">
         <v>20</v>
       </c>
+      <c r="U79" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V79" t="inlineStr">
         <is>
           <t>N</t>
@@ -7773,6 +8008,11 @@
       <c r="R80">
         <v>20</v>
       </c>
+      <c r="U80" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V80" t="inlineStr">
         <is>
           <t>N</t>
@@ -7858,6 +8098,11 @@
       <c r="R81">
         <v>20</v>
       </c>
+      <c r="U81" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V81" t="inlineStr">
         <is>
           <t>N</t>
@@ -7943,6 +8188,11 @@
       <c r="R82">
         <v>50</v>
       </c>
+      <c r="U82" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V82" t="inlineStr">
         <is>
           <t>N</t>
@@ -8028,6 +8278,11 @@
       <c r="R83">
         <v>50</v>
       </c>
+      <c r="U83" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V83" t="inlineStr">
         <is>
           <t>N</t>
@@ -8113,6 +8368,11 @@
       <c r="R84">
         <v>50</v>
       </c>
+      <c r="U84" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V84" t="inlineStr">
         <is>
           <t>N</t>
@@ -8198,6 +8458,11 @@
       <c r="R85">
         <v>30</v>
       </c>
+      <c r="U85" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V85" t="inlineStr">
         <is>
           <t>N</t>
@@ -8283,6 +8548,11 @@
       <c r="R86">
         <v>25</v>
       </c>
+      <c r="U86" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V86" t="inlineStr">
         <is>
           <t>N</t>
@@ -8368,6 +8638,11 @@
       <c r="R87">
         <v>25</v>
       </c>
+      <c r="U87" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V87" t="inlineStr">
         <is>
           <t>N</t>
@@ -8453,6 +8728,11 @@
       <c r="R88">
         <v>25</v>
       </c>
+      <c r="U88" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V88" t="inlineStr">
         <is>
           <t>N</t>
@@ -8538,6 +8818,11 @@
       <c r="R89">
         <v>30</v>
       </c>
+      <c r="U89" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V89" t="inlineStr">
         <is>
           <t>N</t>
@@ -8623,6 +8908,11 @@
       <c r="R90">
         <v>30</v>
       </c>
+      <c r="U90" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V90" t="inlineStr">
         <is>
           <t>N</t>
@@ -8708,6 +8998,11 @@
       <c r="R91">
         <v>50</v>
       </c>
+      <c r="U91" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V91" t="inlineStr">
         <is>
           <t>N</t>
@@ -8793,6 +9088,11 @@
       <c r="R92">
         <v>50</v>
       </c>
+      <c r="U92" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V92" t="inlineStr">
         <is>
           <t>N</t>
@@ -8878,6 +9178,11 @@
       <c r="R93">
         <v>50</v>
       </c>
+      <c r="U93" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V93" t="inlineStr">
         <is>
           <t>N</t>
@@ -8963,6 +9268,11 @@
       <c r="R94">
         <v>30</v>
       </c>
+      <c r="U94" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V94" t="inlineStr">
         <is>
           <t>N</t>
@@ -9048,6 +9358,11 @@
       <c r="R95">
         <v>30</v>
       </c>
+      <c r="U95" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V95" t="inlineStr">
         <is>
           <t>N</t>
@@ -9133,6 +9448,11 @@
       <c r="R96">
         <v>30</v>
       </c>
+      <c r="U96" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V96" t="inlineStr">
         <is>
           <t>N</t>
@@ -9218,6 +9538,11 @@
       <c r="R97">
         <v>30</v>
       </c>
+      <c r="U97" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V97" t="inlineStr">
         <is>
           <t>N</t>
@@ -9303,6 +9628,11 @@
       <c r="R98">
         <v>30</v>
       </c>
+      <c r="U98" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V98" t="inlineStr">
         <is>
           <t>N</t>
@@ -9388,6 +9718,11 @@
       <c r="R99">
         <v>30</v>
       </c>
+      <c r="U99" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V99" t="inlineStr">
         <is>
           <t>N</t>
@@ -9473,6 +9808,11 @@
       <c r="R100">
         <v>30</v>
       </c>
+      <c r="U100" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V100" t="inlineStr">
         <is>
           <t>N</t>
@@ -9558,6 +9898,11 @@
       <c r="R101">
         <v>30</v>
       </c>
+      <c r="U101" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V101" t="inlineStr">
         <is>
           <t>N</t>
@@ -9643,6 +9988,11 @@
       <c r="R102">
         <v>30</v>
       </c>
+      <c r="U102" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V102" t="inlineStr">
         <is>
           <t>N</t>
@@ -9728,6 +10078,11 @@
       <c r="R103">
         <v>30</v>
       </c>
+      <c r="U103" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V103" t="inlineStr">
         <is>
           <t>N</t>
@@ -9813,6 +10168,11 @@
       <c r="R104">
         <v>30</v>
       </c>
+      <c r="U104" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V104" t="inlineStr">
         <is>
           <t>N</t>
@@ -9898,6 +10258,11 @@
       <c r="R105">
         <v>30</v>
       </c>
+      <c r="U105" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V105" t="inlineStr">
         <is>
           <t>N</t>
@@ -9983,6 +10348,11 @@
       <c r="R106">
         <v>30</v>
       </c>
+      <c r="U106" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V106" t="inlineStr">
         <is>
           <t>N</t>
@@ -10068,6 +10438,11 @@
       <c r="R107">
         <v>30</v>
       </c>
+      <c r="U107" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V107" t="inlineStr">
         <is>
           <t>N</t>
@@ -10153,6 +10528,11 @@
       <c r="R108">
         <v>30</v>
       </c>
+      <c r="U108" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V108" t="inlineStr">
         <is>
           <t>N</t>
@@ -10238,6 +10618,11 @@
       <c r="R109">
         <v>30</v>
       </c>
+      <c r="U109" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V109" t="inlineStr">
         <is>
           <t>N</t>
@@ -10323,6 +10708,11 @@
       <c r="R110">
         <v>50</v>
       </c>
+      <c r="U110" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V110" t="inlineStr">
         <is>
           <t>N</t>
@@ -10408,6 +10798,11 @@
       <c r="R111">
         <v>50</v>
       </c>
+      <c r="U111" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V111" t="inlineStr">
         <is>
           <t>N</t>
@@ -10493,6 +10888,11 @@
       <c r="R112">
         <v>50</v>
       </c>
+      <c r="U112" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V112" t="inlineStr">
         <is>
           <t>N</t>
@@ -10578,6 +10978,11 @@
       <c r="R113">
         <v>30</v>
       </c>
+      <c r="U113" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V113" t="inlineStr">
         <is>
           <t>N</t>
@@ -10663,6 +11068,11 @@
       <c r="R114">
         <v>30</v>
       </c>
+      <c r="U114" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V114" t="inlineStr">
         <is>
           <t>N</t>
@@ -10748,6 +11158,11 @@
       <c r="R115">
         <v>30</v>
       </c>
+      <c r="U115" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V115" t="inlineStr">
         <is>
           <t>N</t>
@@ -10833,6 +11248,11 @@
       <c r="R116">
         <v>30</v>
       </c>
+      <c r="U116" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V116" t="inlineStr">
         <is>
           <t>N</t>
@@ -10918,6 +11338,11 @@
       <c r="R117">
         <v>50</v>
       </c>
+      <c r="U117" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V117" t="inlineStr">
         <is>
           <t>N</t>
@@ -11003,6 +11428,11 @@
       <c r="R118">
         <v>50</v>
       </c>
+      <c r="U118" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V118" t="inlineStr">
         <is>
           <t>N</t>
@@ -11088,6 +11518,11 @@
       <c r="R119">
         <v>50</v>
       </c>
+      <c r="U119" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V119" t="inlineStr">
         <is>
           <t>N</t>
@@ -11173,6 +11608,11 @@
       <c r="R120">
         <v>50</v>
       </c>
+      <c r="U120" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V120" t="inlineStr">
         <is>
           <t>N</t>
@@ -11258,6 +11698,11 @@
       <c r="R121">
         <v>50</v>
       </c>
+      <c r="U121" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V121" t="inlineStr">
         <is>
           <t>N</t>
@@ -11343,6 +11788,11 @@
       <c r="R122">
         <v>50</v>
       </c>
+      <c r="U122" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V122" t="inlineStr">
         <is>
           <t>N</t>
@@ -11428,6 +11878,11 @@
       <c r="R123">
         <v>25</v>
       </c>
+      <c r="U123" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V123" t="inlineStr">
         <is>
           <t>N</t>
@@ -11513,6 +11968,11 @@
       <c r="R124">
         <v>25</v>
       </c>
+      <c r="U124" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V124" t="inlineStr">
         <is>
           <t>N</t>
@@ -11598,6 +12058,11 @@
       <c r="R125">
         <v>25</v>
       </c>
+      <c r="U125" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V125" t="inlineStr">
         <is>
           <t>N</t>
@@ -11683,6 +12148,11 @@
       <c r="R126">
         <v>25</v>
       </c>
+      <c r="U126" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V126" t="inlineStr">
         <is>
           <t>N</t>
@@ -11768,6 +12238,11 @@
       <c r="R127">
         <v>25</v>
       </c>
+      <c r="U127" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V127" t="inlineStr">
         <is>
           <t>N</t>
@@ -11853,6 +12328,11 @@
       <c r="R128">
         <v>25</v>
       </c>
+      <c r="U128" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V128" t="inlineStr">
         <is>
           <t>N</t>
@@ -11938,6 +12418,11 @@
       <c r="R129">
         <v>25</v>
       </c>
+      <c r="U129" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V129" t="inlineStr">
         <is>
           <t>N</t>
@@ -12023,6 +12508,11 @@
       <c r="R130">
         <v>25</v>
       </c>
+      <c r="U130" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V130" t="inlineStr">
         <is>
           <t>N</t>
@@ -12108,6 +12598,11 @@
       <c r="R131">
         <v>25</v>
       </c>
+      <c r="U131" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V131" t="inlineStr">
         <is>
           <t>N</t>
@@ -12193,6 +12688,11 @@
       <c r="R132">
         <v>25</v>
       </c>
+      <c r="U132" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V132" t="inlineStr">
         <is>
           <t>N</t>
@@ -12278,6 +12778,11 @@
       <c r="R133">
         <v>25</v>
       </c>
+      <c r="U133" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V133" t="inlineStr">
         <is>
           <t>N</t>
@@ -12363,6 +12868,11 @@
       <c r="R134">
         <v>25</v>
       </c>
+      <c r="U134" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V134" t="inlineStr">
         <is>
           <t>N</t>
@@ -12448,6 +12958,11 @@
       <c r="R135">
         <v>25</v>
       </c>
+      <c r="U135" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V135" t="inlineStr">
         <is>
           <t>N</t>
@@ -12533,6 +13048,11 @@
       <c r="R136">
         <v>25</v>
       </c>
+      <c r="U136" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V136" t="inlineStr">
         <is>
           <t>N</t>
@@ -12618,6 +13138,11 @@
       <c r="R137">
         <v>25</v>
       </c>
+      <c r="U137" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V137" t="inlineStr">
         <is>
           <t>N</t>
@@ -12703,6 +13228,11 @@
       <c r="R138">
         <v>25</v>
       </c>
+      <c r="U138" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V138" t="inlineStr">
         <is>
           <t>N</t>
@@ -12788,6 +13318,11 @@
       <c r="R139">
         <v>25</v>
       </c>
+      <c r="U139" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="V139" t="inlineStr">
         <is>
           <t>N</t>
@@ -12872,6 +13407,11 @@
       </c>
       <c r="R140">
         <v>25</v>
+      </c>
+      <c r="U140" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
       <c r="V140" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Updates to models file including robust non-independence sensitivity tests and publication bias tests - funnel plots and meta regressions.
</commit_message>
<xml_diff>
--- a/Analysis/Comp_all_plant.xlsx
+++ b/Analysis/Comp_all_plant.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA140"/>
+  <dimension ref="A1:AB140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -470,25 +470,30 @@
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
+          <t>Year</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
           <t>Imputed</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>Con_count</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>Trt_count</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>Effect_size</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>Sampling_variance</t>
         </is>
@@ -583,15 +588,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z2">
+      <c r="W2">
+        <v>1994</v>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA2">
         <v>3.499039897232711</v>
       </c>
-      <c r="AA2">
+      <c r="AB2">
         <v>0.5060820050606576</v>
       </c>
     </row>
@@ -684,15 +692,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z3">
+      <c r="W3">
+        <v>1994</v>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA3">
         <v>2.183611364438458</v>
       </c>
-      <c r="AA3">
+      <c r="AB3">
         <v>0.3192039647726197</v>
       </c>
     </row>
@@ -785,15 +796,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z4">
+      <c r="W4">
+        <v>1994</v>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA4">
         <v>1.903799351225588</v>
       </c>
-      <c r="AA4">
+      <c r="AB4">
         <v>0.2906112992431743</v>
       </c>
     </row>
@@ -886,15 +900,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W5" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z5">
+      <c r="W5">
+        <v>1994</v>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA5">
         <v>4.217570710902846</v>
       </c>
-      <c r="AA5">
+      <c r="AB5">
         <v>0.6446975675366385</v>
       </c>
     </row>
@@ -987,15 +1004,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W6" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z6">
+      <c r="W6">
+        <v>1994</v>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA6">
         <v>2.153653128971666</v>
       </c>
-      <c r="AA6">
+      <c r="AB6">
         <v>0.3159555449982362</v>
       </c>
     </row>
@@ -1088,15 +1108,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W7" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z7">
+      <c r="W7">
+        <v>1994</v>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA7">
         <v>1.384951185617706</v>
       </c>
-      <c r="AA7">
+      <c r="AB7">
         <v>0.2479522446635972</v>
       </c>
     </row>
@@ -1189,15 +1212,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W8" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z8">
+      <c r="W8">
+        <v>1994</v>
+      </c>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA8">
         <v>1.073337168853721</v>
       </c>
-      <c r="AA8">
+      <c r="AB8">
         <v>0.2288013169510731</v>
       </c>
     </row>
@@ -1290,15 +1316,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W9" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z9">
+      <c r="W9">
+        <v>1993</v>
+      </c>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA9">
         <v>0.2069541687898287</v>
       </c>
-      <c r="AA9">
+      <c r="AB9">
         <v>0.287243929570696</v>
       </c>
     </row>
@@ -1391,15 +1420,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W10" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z10">
+      <c r="W10">
+        <v>1993</v>
+      </c>
+      <c r="X10" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA10">
         <v>0.2414465302548001</v>
       </c>
-      <c r="AA10">
+      <c r="AB10">
         <v>0.2877963009632886</v>
       </c>
     </row>
@@ -1492,15 +1524,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W11" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z11">
+      <c r="W11">
+        <v>1993</v>
+      </c>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA11">
         <v>0.7609456559391127</v>
       </c>
-      <c r="AA11">
+      <c r="AB11">
         <v>0.3063942246890217</v>
       </c>
     </row>
@@ -1593,15 +1628,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W12" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z12">
+      <c r="W12">
+        <v>1993</v>
+      </c>
+      <c r="X12" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA12">
         <v>0.8676757839099919</v>
       </c>
-      <c r="AA12">
+      <c r="AB12">
         <v>0.3126021880708507</v>
       </c>
     </row>
@@ -1691,15 +1729,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W13" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z13">
+      <c r="W13">
+        <v>1983</v>
+      </c>
+      <c r="X13" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA13">
         <v>1.388114515178266</v>
       </c>
-      <c r="AA13">
+      <c r="AB13">
         <v>0.6204288692030371</v>
       </c>
     </row>
@@ -1789,15 +1830,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W14" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z14">
+      <c r="W14">
+        <v>1983</v>
+      </c>
+      <c r="X14" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA14">
         <v>1.301988300645818</v>
       </c>
-      <c r="AA14">
+      <c r="AB14">
         <v>0.6059483459386616</v>
       </c>
     </row>
@@ -1887,15 +1931,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W15" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z15">
+      <c r="W15">
+        <v>1983</v>
+      </c>
+      <c r="X15" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA15">
         <v>2.068580007240947</v>
       </c>
-      <c r="AA15">
+      <c r="AB15">
         <v>0.7674389528973098</v>
       </c>
     </row>
@@ -1985,15 +2032,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W16" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z16">
+      <c r="W16">
+        <v>1983</v>
+      </c>
+      <c r="X16" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA16">
         <v>3.412219707728246</v>
       </c>
-      <c r="AA16">
+      <c r="AB16">
         <v>1.227702708363065</v>
       </c>
     </row>
@@ -2083,15 +2133,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W17" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z17">
+      <c r="W17">
+        <v>1983</v>
+      </c>
+      <c r="X17" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA17">
         <v>1.118134461824235</v>
       </c>
-      <c r="AA17">
+      <c r="AB17">
         <v>0.5781390421699357</v>
       </c>
     </row>
@@ -2181,15 +2234,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W18" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z18">
+      <c r="W18">
+        <v>1983</v>
+      </c>
+      <c r="X18" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA18">
         <v>1.315029395807548</v>
       </c>
-      <c r="AA18">
+      <c r="AB18">
         <v>0.6080813944898728</v>
       </c>
     </row>
@@ -2282,15 +2338,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W19" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z19">
+      <c r="W19">
+        <v>1993</v>
+      </c>
+      <c r="X19" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA19">
         <v>0.3287390226929189</v>
       </c>
-      <c r="AA19">
+      <c r="AB19">
         <v>0.1013508668130137</v>
       </c>
     </row>
@@ -2383,15 +2442,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W20" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z20">
+      <c r="W20">
+        <v>1993</v>
+      </c>
+      <c r="X20" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA20">
         <v>-0.1095796742309731</v>
       </c>
-      <c r="AA20">
+      <c r="AB20">
         <v>0.1001500963125571</v>
       </c>
     </row>
@@ -2484,15 +2546,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W21" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z21">
+      <c r="W21">
+        <v>1993</v>
+      </c>
+      <c r="X21" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA21">
         <v>-0.1095796742309731</v>
       </c>
-      <c r="AA21">
+      <c r="AB21">
         <v>0.1001500963125571</v>
       </c>
     </row>
@@ -2585,15 +2650,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W22" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z22">
+      <c r="W22">
+        <v>1993</v>
+      </c>
+      <c r="X22" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA22">
         <v>-0.3287390226929189</v>
       </c>
-      <c r="AA22">
+      <c r="AB22">
         <v>0.1013508668130137</v>
       </c>
     </row>
@@ -2686,15 +2754,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W23" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z23">
+      <c r="W23">
+        <v>1993</v>
+      </c>
+      <c r="X23" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA23">
         <v>-0.2191593484619459</v>
       </c>
-      <c r="AA23">
+      <c r="AB23">
         <v>0.1006003852502283</v>
       </c>
     </row>
@@ -2787,15 +2858,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W24" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z24">
+      <c r="W24">
+        <v>1993</v>
+      </c>
+      <c r="X24" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA24">
         <v>0.153411543923362</v>
       </c>
-      <c r="AA24">
+      <c r="AB24">
         <v>0.1002941887726119</v>
       </c>
     </row>
@@ -2888,15 +2962,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W25" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z25">
+      <c r="W25">
+        <v>1993</v>
+      </c>
+      <c r="X25" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA25">
         <v>0.06574780453858375</v>
       </c>
-      <c r="AA25">
+      <c r="AB25">
         <v>0.1000540346725206</v>
       </c>
     </row>
@@ -2989,15 +3066,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W26" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z26">
+      <c r="W26">
+        <v>1993</v>
+      </c>
+      <c r="X26" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA26">
         <v>-0.3725708923853082</v>
       </c>
-      <c r="AA26">
+      <c r="AB26">
         <v>0.1017351133731598</v>
       </c>
     </row>
@@ -3090,15 +3170,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W27" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z27">
+      <c r="W27">
+        <v>1993</v>
+      </c>
+      <c r="X27" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA27">
         <v>0.04383186969238904</v>
       </c>
-      <c r="AA27">
+      <c r="AB27">
         <v>0.1000240154100091</v>
       </c>
     </row>
@@ -3191,15 +3274,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W28" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z28">
+      <c r="W28">
+        <v>1993</v>
+      </c>
+      <c r="X28" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA28">
         <v>-0.3506549575391137</v>
       </c>
-      <c r="AA28">
+      <c r="AB28">
         <v>0.1015369862405845</v>
       </c>
     </row>
@@ -3292,15 +3378,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W29" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z29">
+      <c r="W29">
+        <v>1993</v>
+      </c>
+      <c r="X29" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA29">
         <v>0.1948083097439519</v>
       </c>
-      <c r="AA29">
+      <c r="AB29">
         <v>0.1004743784693162</v>
       </c>
     </row>
@@ -3393,15 +3482,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W30" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z30">
+      <c r="W30">
+        <v>1993</v>
+      </c>
+      <c r="X30" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA30">
         <v>0.1704572710259578</v>
       </c>
-      <c r="AA30">
+      <c r="AB30">
         <v>0.1003631960155702</v>
       </c>
     </row>
@@ -3494,15 +3586,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W31" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z31">
+      <c r="W31">
+        <v>1993</v>
+      </c>
+      <c r="X31" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA31">
         <v>-0.292212464615928</v>
       </c>
-      <c r="AA31">
+      <c r="AB31">
         <v>0.1010673515559614</v>
       </c>
     </row>
@@ -3595,15 +3690,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W32" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z32">
+      <c r="W32">
+        <v>1993</v>
+      </c>
+      <c r="X32" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA32">
         <v>0.2435103871799399</v>
       </c>
-      <c r="AA32">
+      <c r="AB32">
         <v>0.1007412163583066</v>
       </c>
     </row>
@@ -3696,15 +3794,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W33" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z33">
+      <c r="W33">
+        <v>1993</v>
+      </c>
+      <c r="X33" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA33">
         <v>-0.292212464615928</v>
       </c>
-      <c r="AA33">
+      <c r="AB33">
         <v>0.1010673515559614</v>
       </c>
     </row>
@@ -3797,15 +3898,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W34" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z34">
+      <c r="W34">
+        <v>1996</v>
+      </c>
+      <c r="X34" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA34">
         <v>0.4826245546317595</v>
       </c>
-      <c r="AA34">
+      <c r="AB34">
         <v>0.01384787081394263</v>
       </c>
     </row>
@@ -3898,15 +4002,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W35" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z35">
+      <c r="W35">
+        <v>1996</v>
+      </c>
+      <c r="X35" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA35">
         <v>0.7347534624913916</v>
       </c>
-      <c r="AA35">
+      <c r="AB35">
         <v>0.01672152177229408</v>
       </c>
     </row>
@@ -3999,15 +4106,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W36" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z36">
+      <c r="W36">
+        <v>1996</v>
+      </c>
+      <c r="X36" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA36">
         <v>1.283884288361518</v>
       </c>
-      <c r="AA36">
+      <c r="AB36">
         <v>0.01628180671924762</v>
       </c>
     </row>
@@ -4100,15 +4210,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W37" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z37">
+      <c r="W37">
+        <v>1996</v>
+      </c>
+      <c r="X37" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA37">
         <v>1.497532393138095</v>
       </c>
-      <c r="AA37">
+      <c r="AB37">
         <v>0.08535502723748258</v>
       </c>
     </row>
@@ -4201,15 +4314,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W38" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z38">
+      <c r="W38">
+        <v>1996</v>
+      </c>
+      <c r="X38" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA38">
         <v>2.650369579498177</v>
       </c>
-      <c r="AA38">
+      <c r="AB38">
         <v>0.1252038242327445</v>
       </c>
     </row>
@@ -4302,15 +4418,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W39" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z39">
+      <c r="W39">
+        <v>1996</v>
+      </c>
+      <c r="X39" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA39">
         <v>4.664932437688604</v>
       </c>
-      <c r="AA39">
+      <c r="AB39">
         <v>0.2480132887349945</v>
       </c>
     </row>
@@ -4403,15 +4522,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W40" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z40">
+      <c r="W40">
+        <v>1996</v>
+      </c>
+      <c r="X40" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA40">
         <v>1.142026616055801</v>
       </c>
-      <c r="AA40">
+      <c r="AB40">
         <v>0.07753520659816554</v>
       </c>
     </row>
@@ -4504,15 +4626,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W41" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z41">
+      <c r="W41">
+        <v>1996</v>
+      </c>
+      <c r="X41" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA41">
         <v>1.312509403923769</v>
       </c>
-      <c r="AA41">
+      <c r="AB41">
         <v>0.08102234112823607</v>
       </c>
     </row>
@@ -4605,15 +4730,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W42" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z42">
+      <c r="W42">
+        <v>1996</v>
+      </c>
+      <c r="X42" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA42">
         <v>2.188842124812699</v>
       </c>
-      <c r="AA42">
+      <c r="AB42">
         <v>0.1065919153946214</v>
       </c>
     </row>
@@ -4706,15 +4834,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W43" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z43">
+      <c r="W43">
+        <v>1996</v>
+      </c>
+      <c r="X43" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA43">
         <v>1.293209869243623</v>
       </c>
-      <c r="AA43">
+      <c r="AB43">
         <v>0.08060326471590923</v>
       </c>
     </row>
@@ -4807,15 +4938,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W44" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z44">
+      <c r="W44">
+        <v>1996</v>
+      </c>
+      <c r="X44" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA44">
         <v>1.500949266816194</v>
       </c>
-      <c r="AA44">
+      <c r="AB44">
         <v>0.08544040584630058</v>
       </c>
     </row>
@@ -4908,15 +5042,18 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W45" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z45">
+      <c r="W45">
+        <v>1996</v>
+      </c>
+      <c r="X45" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA45">
         <v>2.000836224954823</v>
       </c>
-      <c r="AA45">
+      <c r="AB45">
         <v>0.1000278799924289</v>
       </c>
     </row>
@@ -5009,15 +5146,18 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="W46" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z46">
+      <c r="W46">
+        <v>2017</v>
+      </c>
+      <c r="X46" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA46">
         <v>0.4381649613626656</v>
       </c>
-      <c r="AA46">
+      <c r="AB46">
         <v>0.03199995520846072</v>
       </c>
     </row>
@@ -5110,15 +5250,18 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="W47" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z47">
+      <c r="W47">
+        <v>2017</v>
+      </c>
+      <c r="X47" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA47">
         <v>0.5251773910921815</v>
       </c>
-      <c r="AA47">
+      <c r="AB47">
         <v>0.03232738785982184</v>
       </c>
     </row>
@@ -5211,15 +5354,18 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="W48" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z48">
+      <c r="W48">
+        <v>2017</v>
+      </c>
+      <c r="X48" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA48">
         <v>0.6698142574083952</v>
       </c>
-      <c r="AA48">
+      <c r="AB48">
         <v>0.0330025435133889</v>
       </c>
     </row>
@@ -5312,15 +5458,18 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="W49" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z49">
+      <c r="W49">
+        <v>2017</v>
+      </c>
+      <c r="X49" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA49">
         <v>0.5412368926163361</v>
       </c>
-      <c r="AA49">
+      <c r="AB49">
         <v>0.03239428661691011</v>
       </c>
     </row>
@@ -5413,15 +5562,18 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="W50" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z50">
+      <c r="W50">
+        <v>2017</v>
+      </c>
+      <c r="X50" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA50">
         <v>0.5962847511774579</v>
       </c>
-      <c r="AA50">
+      <c r="AB50">
         <v>0.03263888868940142</v>
       </c>
     </row>
@@ -5514,15 +5666,18 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="W51" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z51">
+      <c r="W51">
+        <v>2017</v>
+      </c>
+      <c r="X51" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA51">
         <v>0.2445359007775916</v>
       </c>
-      <c r="AA51">
+      <c r="AB51">
         <v>0.03148358518269183</v>
       </c>
     </row>
@@ -5615,15 +5770,18 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="W52" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z52">
+      <c r="W52">
+        <v>2008</v>
+      </c>
+      <c r="X52" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA52">
         <v>0.1220870312740429</v>
       </c>
-      <c r="AA52">
+      <c r="AB52">
         <v>0.04174429814169432</v>
       </c>
     </row>
@@ -5716,15 +5874,18 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="W53" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z53">
+      <c r="W53">
+        <v>2008</v>
+      </c>
+      <c r="X53" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA53">
         <v>0.1013757313365534</v>
       </c>
-      <c r="AA53">
+      <c r="AB53">
         <v>0.02225076955251117</v>
       </c>
     </row>
@@ -5817,15 +5978,18 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="W54" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z54">
+      <c r="W54">
+        <v>2008</v>
+      </c>
+      <c r="X54" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA54">
         <v>0.1488957394175404</v>
       </c>
-      <c r="AA54">
+      <c r="AB54">
         <v>0.04178213511050363</v>
       </c>
     </row>
@@ -5918,15 +6082,18 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="W55" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z55">
+      <c r="W55">
+        <v>2008</v>
+      </c>
+      <c r="X55" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA55">
         <v>0.1723548896913452</v>
       </c>
-      <c r="AA55">
+      <c r="AB55">
         <v>0.0223047394666681</v>
       </c>
     </row>
@@ -6019,15 +6186,18 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="W56" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z56">
+      <c r="W56">
+        <v>2008</v>
+      </c>
+      <c r="X56" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA56">
         <v>0.3035171078684176</v>
       </c>
-      <c r="AA56">
+      <c r="AB56">
         <v>0.04214647205608754</v>
       </c>
     </row>
@@ -6120,15 +6290,18 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="W57" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z57">
+      <c r="W57">
+        <v>2008</v>
+      </c>
+      <c r="X57" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA57">
         <v>-0.07508464525060481</v>
       </c>
-      <c r="AA57">
+      <c r="AB57">
         <v>0.02223788251097892</v>
       </c>
     </row>
@@ -6221,15 +6394,18 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="W58" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z58">
+      <c r="W58">
+        <v>2008</v>
+      </c>
+      <c r="X58" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA58">
         <v>0.2089652099875066</v>
       </c>
-      <c r="AA58">
+      <c r="AB58">
         <v>0.3351527691243801</v>
       </c>
     </row>
@@ -6322,15 +6498,18 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="W59" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z59">
+      <c r="W59">
+        <v>2008</v>
+      </c>
+      <c r="X59" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA59">
         <v>0.2691758214855794</v>
       </c>
-      <c r="AA59">
+      <c r="AB59">
         <v>0.3363523176196848</v>
       </c>
     </row>
@@ -6423,15 +6602,18 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="W60" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z60">
+      <c r="W60">
+        <v>2008</v>
+      </c>
+      <c r="X60" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA60">
         <v>0.2757660662406149</v>
       </c>
-      <c r="AA60">
+      <c r="AB60">
         <v>0.3365019551370759</v>
       </c>
     </row>
@@ -6524,15 +6706,18 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="W61" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z61">
+      <c r="W61">
+        <v>2008</v>
+      </c>
+      <c r="X61" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA61">
         <v>0.506722938705136</v>
       </c>
-      <c r="AA61">
+      <c r="AB61">
         <v>0.344032005692082</v>
       </c>
     </row>
@@ -6625,15 +6810,18 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="W62" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z62">
+      <c r="W62">
+        <v>2008</v>
+      </c>
+      <c r="X62" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA62">
         <v>1.871451678214122</v>
       </c>
-      <c r="AA62">
+      <c r="AB62">
         <v>0.4792638076621022</v>
       </c>
     </row>
@@ -6726,15 +6914,18 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="W63" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z63">
+      <c r="W63">
+        <v>2008</v>
+      </c>
+      <c r="X63" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA63">
         <v>-1.201102746269639</v>
       </c>
-      <c r="AA63">
+      <c r="AB63">
         <v>0.3934436586290195</v>
       </c>
     </row>
@@ -6827,15 +7018,18 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="W64" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z64">
+      <c r="W64">
+        <v>2008</v>
+      </c>
+      <c r="X64" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA64">
         <v>0.5387328029832621</v>
       </c>
-      <c r="AA64">
+      <c r="AB64">
         <v>0.3454263763754251</v>
       </c>
     </row>
@@ -6928,15 +7122,18 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="W65" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z65">
+      <c r="W65">
+        <v>2008</v>
+      </c>
+      <c r="X65" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA65">
         <v>0.5455385328655102</v>
       </c>
-      <c r="AA65">
+      <c r="AB65">
         <v>0.3457338454517105</v>
       </c>
     </row>
@@ -7029,15 +7226,18 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="W66" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z66">
+      <c r="W66">
+        <v>2008</v>
+      </c>
+      <c r="X66" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA66">
         <v>1.063399065242261</v>
       </c>
-      <c r="AA66">
+      <c r="AB66">
         <v>0.3804507321649214</v>
       </c>
     </row>
@@ -7130,15 +7330,18 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="W67" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z67">
+      <c r="W67">
+        <v>2008</v>
+      </c>
+      <c r="X67" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA67">
         <v>3.177349744814837</v>
       </c>
-      <c r="AA67">
+      <c r="AB67">
         <v>0.7539813083697879</v>
       </c>
     </row>
@@ -7231,15 +7434,18 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="W68" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z68">
+      <c r="W68">
+        <v>2008</v>
+      </c>
+      <c r="X68" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA68">
         <v>-2.666255512156723</v>
       </c>
-      <c r="AA68">
+      <c r="AB68">
         <v>0.6295382690044211</v>
       </c>
     </row>
@@ -7332,15 +7538,18 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="W69" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z69">
+      <c r="W69">
+        <v>2017</v>
+      </c>
+      <c r="X69" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA69">
         <v>0.5148472963970744</v>
       </c>
-      <c r="AA69">
+      <c r="AB69">
         <v>0.516566733662961</v>
       </c>
     </row>
@@ -7433,15 +7642,18 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="W70" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z70">
+      <c r="W70">
+        <v>2017</v>
+      </c>
+      <c r="X70" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA70">
         <v>0.8721145043507317</v>
       </c>
-      <c r="AA70">
+      <c r="AB70">
         <v>0.5475364817936826</v>
       </c>
     </row>
@@ -7534,15 +7746,18 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="W71" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z71">
+      <c r="W71">
+        <v>2017</v>
+      </c>
+      <c r="X71" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA71">
         <v>0.7105402722719777</v>
       </c>
-      <c r="AA71">
+      <c r="AB71">
         <v>0.531554217407521</v>
       </c>
     </row>
@@ -7635,15 +7850,18 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="W72" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z72">
+      <c r="W72">
+        <v>2017</v>
+      </c>
+      <c r="X72" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA72">
         <v>1.161883609751214</v>
       </c>
-      <c r="AA72">
+      <c r="AB72">
         <v>0.584373345163032</v>
       </c>
     </row>
@@ -7736,15 +7954,18 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="W73" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z73">
+      <c r="W73">
+        <v>2017</v>
+      </c>
+      <c r="X73" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA73">
         <v>2.662191284547399</v>
       </c>
-      <c r="AA73">
+      <c r="AB73">
         <v>0.9429539022200083</v>
       </c>
     </row>
@@ -7837,15 +8058,18 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="W74" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z74">
+      <c r="W74">
+        <v>2017</v>
+      </c>
+      <c r="X74" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA74">
         <v>2.187792670802673</v>
       </c>
-      <c r="AA74">
+      <c r="AB74">
         <v>0.7991522981511183</v>
       </c>
     </row>
@@ -7938,15 +8162,18 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="W75" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z75">
+      <c r="W75">
+        <v>2019</v>
+      </c>
+      <c r="X75" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA75">
         <v>0.02682567791462725</v>
       </c>
-      <c r="AA75">
+      <c r="AB75">
         <v>0.400035980849779</v>
       </c>
     </row>
@@ -8039,15 +8266,18 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="W76" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="Z76">
+      <c r="W76">
+        <v>2019</v>
+      </c>
+      <c r="X76" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AA76">
         <v>1.758471971197474</v>
       </c>
-      <c r="AA76">
+      <c r="AB76">
         <v>0.5546111836743565</v>
       </c>
     </row>
@@ -8128,21 +8358,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W77" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X77">
-        <v>16</v>
+      <c r="W77">
+        <v>1993</v>
+      </c>
+      <c r="X77" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
       <c r="Y77">
         <v>16</v>
       </c>
       <c r="Z77">
+        <v>16</v>
+      </c>
+      <c r="AA77">
         <v>-0</v>
       </c>
-      <c r="AA77">
+      <c r="AB77">
         <v>0.1899772193293833</v>
       </c>
     </row>
@@ -8223,21 +8456,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W78" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X78">
-        <v>16</v>
+      <c r="W78">
+        <v>1993</v>
+      </c>
+      <c r="X78" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
       </c>
       <c r="Y78">
         <v>16</v>
       </c>
       <c r="Z78">
+        <v>16</v>
+      </c>
+      <c r="AA78">
         <v>-0</v>
       </c>
-      <c r="AA78">
+      <c r="AB78">
         <v>0.1899772193293833</v>
       </c>
     </row>
@@ -8318,21 +8554,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W79" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X79">
+      <c r="W79">
+        <v>1993</v>
+      </c>
+      <c r="X79" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y79">
         <v>16</v>
       </c>
-      <c r="Y79">
+      <c r="Z79">
         <v>18</v>
       </c>
-      <c r="Z79">
+      <c r="AA79">
         <v>-0.4470892603707035</v>
       </c>
-      <c r="AA79">
+      <c r="AB79">
         <v>0.263857249068588</v>
       </c>
     </row>
@@ -8413,21 +8652,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W80" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X80">
+      <c r="W80">
+        <v>1993</v>
+      </c>
+      <c r="X80" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y80">
         <v>16</v>
       </c>
-      <c r="Y80">
+      <c r="Z80">
         <v>15</v>
       </c>
-      <c r="Z80">
+      <c r="AA80">
         <v>0.1586074392374924</v>
       </c>
-      <c r="AA80">
+      <c r="AB80">
         <v>0.1760455565785619</v>
       </c>
     </row>
@@ -8508,21 +8750,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W81" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X81">
+      <c r="W81">
+        <v>1993</v>
+      </c>
+      <c r="X81" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y81">
         <v>16</v>
       </c>
-      <c r="Y81">
+      <c r="Z81">
         <v>11</v>
       </c>
-      <c r="Z81">
+      <c r="AA81">
         <v>0.6536685859730176</v>
       </c>
-      <c r="AA81">
+      <c r="AB81">
         <v>0.1563953876297449</v>
       </c>
     </row>
@@ -8603,21 +8848,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W82" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X82">
+      <c r="W82">
+        <v>1984</v>
+      </c>
+      <c r="X82" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y82">
         <v>36</v>
       </c>
-      <c r="Y82">
+      <c r="Z82">
         <v>50</v>
       </c>
-      <c r="Z82">
+      <c r="AA82">
         <v>2.035482522753051</v>
       </c>
-      <c r="AA82">
+      <c r="AB82">
         <v>0.6432369541011593</v>
       </c>
     </row>
@@ -8698,21 +8946,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W83" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X83">
+      <c r="W83">
+        <v>1984</v>
+      </c>
+      <c r="X83" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y83">
         <v>36</v>
       </c>
-      <c r="Y83">
+      <c r="Z83">
         <v>50</v>
       </c>
-      <c r="Z83">
+      <c r="AA83">
         <v>2.035482522753051</v>
       </c>
-      <c r="AA83">
+      <c r="AB83">
         <v>0.6432369541011593</v>
       </c>
     </row>
@@ -8793,21 +9044,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W84" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X84">
+      <c r="W84">
+        <v>1984</v>
+      </c>
+      <c r="X84" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y84">
         <v>36</v>
       </c>
-      <c r="Y84">
+      <c r="Z84">
         <v>50</v>
       </c>
-      <c r="Z84">
+      <c r="AA84">
         <v>2.035482522753051</v>
       </c>
-      <c r="AA84">
+      <c r="AB84">
         <v>0.6432369541011593</v>
       </c>
     </row>
@@ -8888,21 +9142,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W85" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X85">
+      <c r="W85">
+        <v>1984</v>
+      </c>
+      <c r="X85" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y85">
         <v>15</v>
       </c>
-      <c r="Y85">
+      <c r="Z85">
         <v>28</v>
       </c>
-      <c r="Z85">
+      <c r="AA85">
         <v>1.454988562491565</v>
       </c>
-      <c r="AA85">
+      <c r="AB85">
         <v>0.203366090024978</v>
       </c>
     </row>
@@ -8983,21 +9240,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W86" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X86">
+      <c r="W86">
+        <v>1984</v>
+      </c>
+      <c r="X86" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y86">
         <v>12</v>
       </c>
-      <c r="Y86">
+      <c r="Z86">
         <v>13</v>
       </c>
-      <c r="Z86">
+      <c r="AA86">
         <v>0.08825971521644058</v>
       </c>
-      <c r="AA86">
+      <c r="AB86">
         <v>0.09742421504070939</v>
       </c>
     </row>
@@ -9078,21 +9338,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W87" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X87">
+      <c r="W87">
+        <v>1984</v>
+      </c>
+      <c r="X87" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y87">
         <v>9</v>
       </c>
-      <c r="Y87">
+      <c r="Z87">
         <v>10</v>
       </c>
-      <c r="Z87">
+      <c r="AA87">
         <v>0.09367024828963293</v>
       </c>
-      <c r="AA87">
+      <c r="AB87">
         <v>0.1034320416348865</v>
       </c>
     </row>
@@ -9173,21 +9436,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W88" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X88">
+      <c r="W88">
+        <v>1984</v>
+      </c>
+      <c r="X88" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y88">
         <v>9</v>
       </c>
-      <c r="Y88">
+      <c r="Z88">
         <v>10</v>
       </c>
-      <c r="Z88">
+      <c r="AA88">
         <v>0.09367024828963293</v>
       </c>
-      <c r="AA88">
+      <c r="AB88">
         <v>0.1034320416348865</v>
       </c>
     </row>
@@ -9268,21 +9534,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W89" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X89">
+      <c r="W89">
+        <v>1984</v>
+      </c>
+      <c r="X89" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y89">
         <v>2</v>
       </c>
-      <c r="Y89">
+      <c r="Z89">
         <v>29</v>
       </c>
-      <c r="Z89">
+      <c r="AA89">
         <v>3.311476052996414</v>
       </c>
-      <c r="AA89">
+      <c r="AB89">
         <v>0.4772826692511602</v>
       </c>
     </row>
@@ -9363,21 +9632,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W90" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X90">
+      <c r="W90">
+        <v>1984</v>
+      </c>
+      <c r="X90" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y90">
         <v>2</v>
       </c>
-      <c r="Y90">
+      <c r="Z90">
         <v>30</v>
       </c>
-      <c r="Z90">
+      <c r="AA90">
         <v>3.608164909869637</v>
       </c>
-      <c r="AA90">
+      <c r="AB90">
         <v>0.7501439280398378</v>
       </c>
     </row>
@@ -9458,21 +9730,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W91" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X91">
+      <c r="W91">
+        <v>1984</v>
+      </c>
+      <c r="X91" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y91">
         <v>3</v>
       </c>
-      <c r="Y91">
+      <c r="Z91">
         <v>29</v>
       </c>
-      <c r="Z91">
+      <c r="AA91">
         <v>1.694955222681405</v>
       </c>
-      <c r="AA91">
+      <c r="AB91">
         <v>0.1327444497986817</v>
       </c>
     </row>
@@ -9553,21 +9828,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W92" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X92">
+      <c r="W92">
+        <v>1984</v>
+      </c>
+      <c r="X92" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y92">
         <v>3</v>
       </c>
-      <c r="Y92">
+      <c r="Z92">
         <v>38</v>
       </c>
-      <c r="Z92">
+      <c r="AA92">
         <v>2.152506445843135</v>
       </c>
-      <c r="AA92">
+      <c r="AB92">
         <v>0.1411178299609828</v>
       </c>
     </row>
@@ -9648,21 +9926,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W93" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X93">
+      <c r="W93">
+        <v>1984</v>
+      </c>
+      <c r="X93" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y93">
         <v>3</v>
       </c>
-      <c r="Y93">
+      <c r="Z93">
         <v>50</v>
       </c>
-      <c r="Z93">
+      <c r="AA93">
         <v>3.982296720252773</v>
       </c>
-      <c r="AA93">
+      <c r="AB93">
         <v>0.7071921435577877</v>
       </c>
     </row>
@@ -9743,21 +10024,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W94" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X94">
+      <c r="W94">
+        <v>1984</v>
+      </c>
+      <c r="X94" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y94">
         <v>2</v>
       </c>
-      <c r="Y94">
+      <c r="Z94">
         <v>28</v>
       </c>
-      <c r="Z94">
+      <c r="AA94">
         <v>2.909977124983129</v>
       </c>
-      <c r="AA94">
+      <c r="AB94">
         <v>0.3256752331360857</v>
       </c>
     </row>
@@ -9838,21 +10122,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W95" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X95">
+      <c r="W95">
+        <v>1984</v>
+      </c>
+      <c r="X95" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y95">
         <v>1</v>
       </c>
-      <c r="Y95">
+      <c r="Z95">
         <v>6</v>
       </c>
-      <c r="Z95">
+      <c r="AA95">
         <v>1.092183351659161</v>
       </c>
-      <c r="AA95">
+      <c r="AB95">
         <v>0.3777707924595783</v>
       </c>
     </row>
@@ -9933,21 +10220,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W96" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X96">
+      <c r="W96">
+        <v>1984</v>
+      </c>
+      <c r="X96" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y96">
         <v>1</v>
       </c>
-      <c r="Y96">
+      <c r="Z96">
         <v>29</v>
       </c>
-      <c r="Z96">
+      <c r="AA96">
         <v>3.712974981009698</v>
       </c>
-      <c r="AA96">
+      <c r="AB96">
         <v>0.6288901053662344</v>
       </c>
     </row>
@@ -10028,21 +10318,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W97" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X97">
+      <c r="W97">
+        <v>1984</v>
+      </c>
+      <c r="X97" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y97">
         <v>0</v>
       </c>
-      <c r="Y97">
+      <c r="Z97">
         <v>27</v>
       </c>
-      <c r="Z97">
+      <c r="AA97">
         <v>3.402965632285575</v>
       </c>
-      <c r="AA97">
+      <c r="AB97">
         <v>0.7157930687872066</v>
       </c>
     </row>
@@ -10123,21 +10416,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W98" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X98">
+      <c r="W98">
+        <v>1984</v>
+      </c>
+      <c r="X98" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y98">
         <v>0</v>
       </c>
-      <c r="Y98">
+      <c r="Z98">
         <v>25</v>
       </c>
-      <c r="Z98">
+      <c r="AA98">
         <v>3.112143677744915</v>
       </c>
-      <c r="AA98">
+      <c r="AB98">
         <v>0.6850793593377951</v>
       </c>
     </row>
@@ -10218,21 +10514,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W99" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X99">
+      <c r="W99">
+        <v>1984</v>
+      </c>
+      <c r="X99" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y99">
         <v>0</v>
       </c>
-      <c r="Y99">
+      <c r="Z99">
         <v>21</v>
       </c>
-      <c r="Z99">
+      <c r="AA99">
         <v>2.716747561977932</v>
       </c>
-      <c r="AA99">
+      <c r="AB99">
         <v>0.6640271227506831</v>
       </c>
     </row>
@@ -10313,21 +10612,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W100" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X100">
+      <c r="W100">
+        <v>1984</v>
+      </c>
+      <c r="X100" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y100">
         <v>0</v>
       </c>
-      <c r="Y100">
+      <c r="Z100">
         <v>22</v>
       </c>
-      <c r="Z100">
+      <c r="AA100">
         <v>2.803134189008829</v>
       </c>
-      <c r="AA100">
+      <c r="AB100">
         <v>0.6671630288256383</v>
       </c>
     </row>
@@ -10408,21 +10710,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W101" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X101">
+      <c r="W101">
+        <v>1984</v>
+      </c>
+      <c r="X101" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y101">
         <v>0</v>
       </c>
-      <c r="Y101">
+      <c r="Z101">
         <v>11</v>
       </c>
-      <c r="Z101">
+      <c r="AA101">
         <v>1.975304713752321</v>
       </c>
-      <c r="AA101">
+      <c r="AB101">
         <v>0.6599126074478092</v>
       </c>
     </row>
@@ -10503,21 +10808,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W102" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X102">
+      <c r="W102">
+        <v>1984</v>
+      </c>
+      <c r="X102" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y102">
         <v>0</v>
       </c>
-      <c r="Y102">
+      <c r="Z102">
         <v>5</v>
       </c>
-      <c r="Z102">
+      <c r="AA102">
         <v>1.420743415761057</v>
       </c>
-      <c r="AA102">
+      <c r="AB102">
         <v>0.6850793593377951</v>
       </c>
     </row>
@@ -10598,21 +10906,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W103" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X103">
+      <c r="W103">
+        <v>1984</v>
+      </c>
+      <c r="X103" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y103">
         <v>0</v>
       </c>
-      <c r="Y103">
+      <c r="Z103">
         <v>17</v>
       </c>
-      <c r="Z103">
+      <c r="AA103">
         <v>2.409519567509366</v>
       </c>
-      <c r="AA103">
+      <c r="AB103">
         <v>0.6577782842716516</v>
       </c>
     </row>
@@ -10693,21 +11004,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W104" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X104">
+      <c r="W104">
+        <v>1984</v>
+      </c>
+      <c r="X104" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y104">
         <v>0</v>
       </c>
-      <c r="Y104">
+      <c r="Z104">
         <v>30</v>
       </c>
-      <c r="Z104">
+      <c r="AA104">
         <v>4.532887093505972</v>
       </c>
-      <c r="AA104">
+      <c r="AB104">
         <v>1.235786239834415</v>
       </c>
     </row>
@@ -10788,21 +11102,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W105" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X105">
+      <c r="W105">
+        <v>1984</v>
+      </c>
+      <c r="X105" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y105">
         <v>0</v>
       </c>
-      <c r="Y105">
+      <c r="Z105">
         <v>10</v>
       </c>
-      <c r="Z105">
+      <c r="AA105">
         <v>1.897577153824595</v>
       </c>
-      <c r="AA105">
+      <c r="AB105">
         <v>0.6616695198184266</v>
       </c>
     </row>
@@ -10883,21 +11200,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W106" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X106">
+      <c r="W106">
+        <v>1984</v>
+      </c>
+      <c r="X106" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y106">
         <v>0</v>
       </c>
-      <c r="Y106">
+      <c r="Z106">
         <v>24</v>
       </c>
-      <c r="Z106">
+      <c r="AA106">
         <v>2.997985836828322</v>
       </c>
-      <c r="AA106">
+      <c r="AB106">
         <v>0.6770634186847893</v>
       </c>
     </row>
@@ -10978,21 +11298,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W107" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X107">
+      <c r="W107">
+        <v>1984</v>
+      </c>
+      <c r="X107" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y107">
         <v>0</v>
       </c>
-      <c r="Y107">
+      <c r="Z107">
         <v>19</v>
       </c>
-      <c r="Z107">
+      <c r="AA107">
         <v>2.55758237975365</v>
       </c>
-      <c r="AA107">
+      <c r="AB107">
         <v>0.6599126074478092</v>
       </c>
     </row>
@@ -11073,21 +11396,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W108" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X108">
+      <c r="W108">
+        <v>1984</v>
+      </c>
+      <c r="X108" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y108">
         <v>0</v>
       </c>
-      <c r="Y108">
+      <c r="Z108">
         <v>8</v>
       </c>
-      <c r="Z108">
+      <c r="AA108">
         <v>1.729752904497142</v>
       </c>
-      <c r="AA108">
+      <c r="AB108">
         <v>0.6671630288256383</v>
       </c>
     </row>
@@ -11168,21 +11494,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W109" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X109">
+      <c r="W109">
+        <v>1984</v>
+      </c>
+      <c r="X109" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y109">
         <v>0</v>
       </c>
-      <c r="Y109">
+      <c r="Z109">
         <v>30</v>
       </c>
-      <c r="Z109">
+      <c r="AA109">
         <v>4.532887093505972</v>
       </c>
-      <c r="AA109">
+      <c r="AB109">
         <v>1.235786239834415</v>
       </c>
     </row>
@@ -11263,21 +11592,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W110" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X110">
+      <c r="W110">
+        <v>1984</v>
+      </c>
+      <c r="X110" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y110">
         <v>0</v>
       </c>
-      <c r="Y110">
+      <c r="Z110">
         <v>27</v>
       </c>
-      <c r="Z110">
+      <c r="AA110">
         <v>2.631110250928183</v>
       </c>
-      <c r="AA110">
+      <c r="AB110">
         <v>0.6379340212924963</v>
       </c>
     </row>
@@ -11358,21 +11690,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W111" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X111">
+      <c r="W111">
+        <v>1984</v>
+      </c>
+      <c r="X111" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y111">
         <v>0</v>
       </c>
-      <c r="Y111">
+      <c r="Z111">
         <v>39</v>
       </c>
-      <c r="Z111">
+      <c r="AA111">
         <v>3.22476359222267</v>
       </c>
-      <c r="AA111">
+      <c r="AB111">
         <v>0.6480730749647954</v>
       </c>
     </row>
@@ -11453,21 +11788,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W112" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X112">
+      <c r="W112">
+        <v>1984</v>
+      </c>
+      <c r="X112" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y112">
         <v>0</v>
       </c>
-      <c r="Y112">
+      <c r="Z112">
         <v>50</v>
       </c>
-      <c r="Z112">
+      <c r="AA112">
         <v>5.088898593577085</v>
       </c>
-      <c r="AA112">
+      <c r="AB112">
         <v>1.227892364140806</v>
       </c>
     </row>
@@ -11548,21 +11886,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W113" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X113">
+      <c r="W113">
+        <v>1984</v>
+      </c>
+      <c r="X113" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y113">
         <v>0</v>
       </c>
-      <c r="Y113">
+      <c r="Z113">
         <v>30</v>
       </c>
-      <c r="Z113">
+      <c r="AA113">
         <v>4.532887093505972</v>
       </c>
-      <c r="AA113">
+      <c r="AB113">
         <v>1.235786239834415</v>
       </c>
     </row>
@@ -11643,21 +11984,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W114" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X114">
+      <c r="W114">
+        <v>1984</v>
+      </c>
+      <c r="X114" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y114">
         <v>0</v>
       </c>
-      <c r="Y114">
+      <c r="Z114">
         <v>5</v>
       </c>
-      <c r="Z114">
+      <c r="AA114">
         <v>1.420743415761057</v>
       </c>
-      <c r="AA114">
+      <c r="AB114">
         <v>0.6850793593377951</v>
       </c>
     </row>
@@ -11738,21 +12082,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W115" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X115">
+      <c r="W115">
+        <v>1984</v>
+      </c>
+      <c r="X115" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y115">
         <v>0</v>
       </c>
-      <c r="Y115">
+      <c r="Z115">
         <v>21</v>
       </c>
-      <c r="Z115">
+      <c r="AA115">
         <v>2.716747561977932</v>
       </c>
-      <c r="AA115">
+      <c r="AB115">
         <v>0.6640271227506831</v>
       </c>
     </row>
@@ -11833,21 +12180,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W116" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X116">
+      <c r="W116">
+        <v>1984</v>
+      </c>
+      <c r="X116" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y116">
         <v>0</v>
       </c>
-      <c r="Y116">
+      <c r="Z116">
         <v>13</v>
       </c>
-      <c r="Z116">
+      <c r="AA116">
         <v>2.123367525996605</v>
       </c>
-      <c r="AA116">
+      <c r="AB116">
         <v>0.6577782842716516</v>
       </c>
     </row>
@@ -11928,21 +12278,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W117" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X117">
+      <c r="W117">
+        <v>1985</v>
+      </c>
+      <c r="X117" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y117">
         <v>41</v>
       </c>
-      <c r="Y117">
+      <c r="Z117">
         <v>50</v>
       </c>
-      <c r="Z117">
+      <c r="AA117">
         <v>1.731569075467788</v>
       </c>
-      <c r="AA117">
+      <c r="AB117">
         <v>0.6532667682397821</v>
       </c>
     </row>
@@ -12023,21 +12376,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W118" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X118">
+      <c r="W118">
+        <v>1985</v>
+      </c>
+      <c r="X118" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y118">
         <v>41</v>
       </c>
-      <c r="Y118">
+      <c r="Z118">
         <v>49</v>
       </c>
-      <c r="Z118">
+      <c r="AA118">
         <v>1.309666799748525</v>
       </c>
-      <c r="AA118">
+      <c r="AB118">
         <v>0.3513543617263746</v>
       </c>
     </row>
@@ -12118,21 +12474,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W119" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X119">
+      <c r="W119">
+        <v>1985</v>
+      </c>
+      <c r="X119" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y119">
         <v>8</v>
       </c>
-      <c r="Y119">
+      <c r="Z119">
         <v>38</v>
       </c>
-      <c r="Z119">
+      <c r="AA119">
         <v>1.549734574820891</v>
       </c>
-      <c r="AA119">
+      <c r="AB119">
         <v>0.07856200799335403</v>
       </c>
     </row>
@@ -12213,21 +12572,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W120" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X120">
+      <c r="W120">
+        <v>1985</v>
+      </c>
+      <c r="X120" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y120">
         <v>8</v>
       </c>
-      <c r="Y120">
+      <c r="Z120">
         <v>0</v>
       </c>
-      <c r="Z120">
+      <c r="AA120">
         <v>-1.657119670276294</v>
       </c>
-      <c r="AA120">
+      <c r="AB120">
         <v>0.6568586833777462</v>
       </c>
     </row>
@@ -12308,21 +12670,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W121" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X121">
+      <c r="W121">
+        <v>1985</v>
+      </c>
+      <c r="X121" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y121">
         <v>6</v>
       </c>
-      <c r="Y121">
+      <c r="Z121">
         <v>8</v>
       </c>
-      <c r="Z121">
+      <c r="AA121">
         <v>0.1842552680724825</v>
       </c>
-      <c r="AA121">
+      <c r="AB121">
         <v>0.1028015256111382</v>
       </c>
     </row>
@@ -12403,21 +12768,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W122" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X122">
+      <c r="W122">
+        <v>1985</v>
+      </c>
+      <c r="X122" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y122">
         <v>6</v>
       </c>
-      <c r="Y122">
+      <c r="Z122">
         <v>0</v>
       </c>
-      <c r="Z122">
+      <c r="AA122">
         <v>-1.483865061176143</v>
       </c>
-      <c r="AA122">
+      <c r="AB122">
         <v>0.6675404468838091</v>
       </c>
     </row>
@@ -12498,21 +12866,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W123" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X123">
+      <c r="W123">
+        <v>1991</v>
+      </c>
+      <c r="X123" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y123">
         <v>36</v>
       </c>
-      <c r="Y123">
+      <c r="Z123">
         <v>12</v>
       </c>
-      <c r="Z123">
+      <c r="AA123">
         <v>0.7463439547829011</v>
       </c>
-      <c r="AA123">
+      <c r="AB123">
         <v>0.05916854313907278</v>
       </c>
     </row>
@@ -12593,21 +12964,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W124" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X124">
+      <c r="W124">
+        <v>1991</v>
+      </c>
+      <c r="X124" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y124">
         <v>36</v>
       </c>
-      <c r="Y124">
+      <c r="Z124">
         <v>18</v>
       </c>
-      <c r="Z124">
+      <c r="AA124">
         <v>1.311182787961636</v>
       </c>
-      <c r="AA124">
+      <c r="AB124">
         <v>0.07076666397725247</v>
       </c>
     </row>
@@ -12688,21 +13062,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W125" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X125">
+      <c r="W125">
+        <v>1991</v>
+      </c>
+      <c r="X125" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y125">
         <v>12</v>
       </c>
-      <c r="Y125">
+      <c r="Z125">
         <v>5</v>
       </c>
-      <c r="Z125">
+      <c r="AA125">
         <v>0.7131907687936432</v>
       </c>
-      <c r="AA125">
+      <c r="AB125">
         <v>0.1030581182190636</v>
       </c>
     </row>
@@ -12783,21 +13160,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W126" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X126">
+      <c r="W126">
+        <v>1991</v>
+      </c>
+      <c r="X126" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y126">
         <v>12</v>
       </c>
-      <c r="Y126">
+      <c r="Z126">
         <v>11</v>
       </c>
-      <c r="Z126">
+      <c r="AA126">
         <v>1.344535297236829</v>
       </c>
-      <c r="AA126">
+      <c r="AB126">
         <v>0.07641196278065655</v>
       </c>
     </row>
@@ -12878,21 +13258,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W127" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X127">
+      <c r="W127">
+        <v>1991</v>
+      </c>
+      <c r="X127" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y127">
         <v>7</v>
       </c>
-      <c r="Y127">
+      <c r="Z127">
         <v>6</v>
       </c>
-      <c r="Z127">
+      <c r="AA127">
         <v>1.154685150515944</v>
       </c>
-      <c r="AA127">
+      <c r="AB127">
         <v>0.1117707242610901</v>
       </c>
     </row>
@@ -12973,21 +13356,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W128" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X128">
+      <c r="W128">
+        <v>1991</v>
+      </c>
+      <c r="X128" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y128">
         <v>7</v>
       </c>
-      <c r="Y128">
+      <c r="Z128">
         <v>21</v>
       </c>
-      <c r="Z128">
+      <c r="AA128">
         <v>2.704419725336835</v>
       </c>
-      <c r="AA128">
+      <c r="AB128">
         <v>0.1355773933499853</v>
       </c>
     </row>
@@ -13068,21 +13454,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W129" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X129">
+      <c r="W129">
+        <v>1991</v>
+      </c>
+      <c r="X129" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y129">
         <v>7</v>
       </c>
-      <c r="Y129">
+      <c r="Z129">
         <v>3</v>
       </c>
-      <c r="Z129">
+      <c r="AA129">
         <v>0.691706349601896</v>
       </c>
-      <c r="AA129">
+      <c r="AB129">
         <v>0.1602497594966585</v>
       </c>
     </row>
@@ -13163,21 +13552,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W130" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X130">
+      <c r="W130">
+        <v>1991</v>
+      </c>
+      <c r="X130" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y130">
         <v>7</v>
       </c>
-      <c r="Y130">
+      <c r="Z130">
         <v>24</v>
       </c>
-      <c r="Z130">
+      <c r="AA130">
         <v>3.542343579382334</v>
       </c>
-      <c r="AA130">
+      <c r="AB130">
         <v>0.3617407496944893</v>
       </c>
     </row>
@@ -13258,21 +13650,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W131" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X131">
+      <c r="W131">
+        <v>1991</v>
+      </c>
+      <c r="X131" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y131">
         <v>2</v>
       </c>
-      <c r="Y131">
+      <c r="Z131">
         <v>1</v>
       </c>
-      <c r="Z131">
+      <c r="AA131">
         <v>0.7438280334495783</v>
       </c>
-      <c r="AA131">
+      <c r="AB131">
         <v>0.4702535205670393</v>
       </c>
     </row>
@@ -13353,21 +13748,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W132" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X132">
+      <c r="W132">
+        <v>1991</v>
+      </c>
+      <c r="X132" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y132">
         <v>2</v>
       </c>
-      <c r="Y132">
+      <c r="Z132">
         <v>5</v>
       </c>
-      <c r="Z132">
+      <c r="AA132">
         <v>1.731676802480618</v>
       </c>
-      <c r="AA132">
+      <c r="AB132">
         <v>0.2296157094164871</v>
       </c>
     </row>
@@ -13448,21 +13846,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W133" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X133">
+      <c r="W133">
+        <v>1991</v>
+      </c>
+      <c r="X133" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y133">
         <v>1</v>
       </c>
-      <c r="Y133">
+      <c r="Z133">
         <v>0</v>
       </c>
-      <c r="Z133">
+      <c r="AA133">
         <v>0.4913115065665589</v>
       </c>
-      <c r="AA133">
+      <c r="AB133">
         <v>0.8241194397630047</v>
       </c>
     </row>
@@ -13543,21 +13944,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W134" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X134">
+      <c r="W134">
+        <v>1991</v>
+      </c>
+      <c r="X134" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y134">
         <v>1</v>
       </c>
-      <c r="Y134">
+      <c r="Z134">
         <v>15</v>
       </c>
-      <c r="Z134">
+      <c r="AA134">
         <v>3.104649771557755</v>
       </c>
-      <c r="AA134">
+      <c r="AB134">
         <v>0.3562583553875748</v>
       </c>
     </row>
@@ -13638,21 +14042,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W135" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X135">
+      <c r="W135">
+        <v>1991</v>
+      </c>
+      <c r="X135" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y135">
         <v>1</v>
       </c>
-      <c r="Y135">
+      <c r="Z135">
         <v>0</v>
       </c>
-      <c r="Z135">
+      <c r="AA135">
         <v>0.4913115065665589</v>
       </c>
-      <c r="AA135">
+      <c r="AB135">
         <v>0.8241194397630047</v>
       </c>
     </row>
@@ -13733,21 +14140,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W136" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X136">
+      <c r="W136">
+        <v>1991</v>
+      </c>
+      <c r="X136" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y136">
         <v>1</v>
       </c>
-      <c r="Y136">
+      <c r="Z136">
         <v>24</v>
       </c>
-      <c r="Z136">
+      <c r="AA136">
         <v>4.633258049249131</v>
       </c>
-      <c r="AA136">
+      <c r="AB136">
         <v>0.6222264624487116</v>
       </c>
     </row>
@@ -13828,21 +14238,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W137" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X137">
+      <c r="W137">
+        <v>1991</v>
+      </c>
+      <c r="X137" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y137">
         <v>1</v>
       </c>
-      <c r="Y137">
+      <c r="Z137">
         <v>0</v>
       </c>
-      <c r="Z137">
+      <c r="AA137">
         <v>0.4913115065665589</v>
       </c>
-      <c r="AA137">
+      <c r="AB137">
         <v>0.8241194397630047</v>
       </c>
     </row>
@@ -13923,21 +14336,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W138" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X138">
+      <c r="W138">
+        <v>1991</v>
+      </c>
+      <c r="X138" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y138">
         <v>1</v>
       </c>
-      <c r="Y138">
+      <c r="Z138">
         <v>9</v>
       </c>
-      <c r="Z138">
+      <c r="AA138">
         <v>2.563890262897419</v>
       </c>
-      <c r="AA138">
+      <c r="AB138">
         <v>0.3583692133801235</v>
       </c>
     </row>
@@ -14018,21 +14434,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W139" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X139">
+      <c r="W139">
+        <v>1991</v>
+      </c>
+      <c r="X139" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y139">
         <v>1</v>
       </c>
-      <c r="Y139">
+      <c r="Z139">
         <v>0</v>
       </c>
-      <c r="Z139">
+      <c r="AA139">
         <v>0.4913115065665589</v>
       </c>
-      <c r="AA139">
+      <c r="AB139">
         <v>0.8241194397630047</v>
       </c>
     </row>
@@ -14113,21 +14532,24 @@
           <t>N</t>
         </is>
       </c>
-      <c r="W140" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="X140">
+      <c r="W140">
+        <v>1991</v>
+      </c>
+      <c r="X140" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="Y140">
         <v>1</v>
       </c>
-      <c r="Y140">
+      <c r="Z140">
         <v>20</v>
       </c>
-      <c r="Z140">
+      <c r="AA140">
         <v>3.645409280218092</v>
       </c>
-      <c r="AA140">
+      <c r="AB140">
         <v>0.3815886512981592</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Run prelim process with final data set - set seed for imputation for reproducibility
</commit_message>
<xml_diff>
--- a/Analysis/Comp_all_plant.xlsx
+++ b/Analysis/Comp_all_plant.xlsx
@@ -1229,7 +1229,7 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -1333,7 +1333,7 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1437,7 +1437,7 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1541,7 +1541,7 @@
     </row>
     <row r="12">
       <c r="A12">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1645,7 +1645,7 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1746,7 +1746,7 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1847,7 +1847,7 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1948,7 +1948,7 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -2049,7 +2049,7 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -2150,7 +2150,7 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -2251,7 +2251,7 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -2355,7 +2355,7 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -2459,7 +2459,7 @@
     </row>
     <row r="21">
       <c r="A21">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -2563,7 +2563,7 @@
     </row>
     <row r="22">
       <c r="A22">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -2667,7 +2667,7 @@
     </row>
     <row r="23">
       <c r="A23">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -2771,7 +2771,7 @@
     </row>
     <row r="24">
       <c r="A24">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -2875,7 +2875,7 @@
     </row>
     <row r="25">
       <c r="A25">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -2979,7 +2979,7 @@
     </row>
     <row r="26">
       <c r="A26">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -3083,7 +3083,7 @@
     </row>
     <row r="27">
       <c r="A27">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -3187,7 +3187,7 @@
     </row>
     <row r="28">
       <c r="A28">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -3291,7 +3291,7 @@
     </row>
     <row r="29">
       <c r="A29">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -3395,7 +3395,7 @@
     </row>
     <row r="30">
       <c r="A30">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -3499,7 +3499,7 @@
     </row>
     <row r="31">
       <c r="A31">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -3603,7 +3603,7 @@
     </row>
     <row r="32">
       <c r="A32">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -3707,7 +3707,7 @@
     </row>
     <row r="33">
       <c r="A33">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -3811,7 +3811,7 @@
     </row>
     <row r="34">
       <c r="A34">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -3915,7 +3915,7 @@
     </row>
     <row r="35">
       <c r="A35">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -4019,7 +4019,7 @@
     </row>
     <row r="36">
       <c r="A36">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -4123,7 +4123,7 @@
     </row>
     <row r="37">
       <c r="A37">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -4227,7 +4227,7 @@
     </row>
     <row r="38">
       <c r="A38">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -4331,7 +4331,7 @@
     </row>
     <row r="39">
       <c r="A39">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
@@ -4435,7 +4435,7 @@
     </row>
     <row r="40">
       <c r="A40">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -4539,7 +4539,7 @@
     </row>
     <row r="41">
       <c r="A41">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
@@ -4643,7 +4643,7 @@
     </row>
     <row r="42">
       <c r="A42">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
@@ -4747,7 +4747,7 @@
     </row>
     <row r="43">
       <c r="A43">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -4851,7 +4851,7 @@
     </row>
     <row r="44">
       <c r="A44">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -4955,7 +4955,7 @@
     </row>
     <row r="45">
       <c r="A45">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -5059,7 +5059,7 @@
     </row>
     <row r="46">
       <c r="A46">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
@@ -5163,7 +5163,7 @@
     </row>
     <row r="47">
       <c r="A47">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
@@ -5267,7 +5267,7 @@
     </row>
     <row r="48">
       <c r="A48">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
@@ -5371,7 +5371,7 @@
     </row>
     <row r="49">
       <c r="A49">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
@@ -5475,7 +5475,7 @@
     </row>
     <row r="50">
       <c r="A50">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
@@ -5579,7 +5579,7 @@
     </row>
     <row r="51">
       <c r="A51">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
@@ -5683,7 +5683,7 @@
     </row>
     <row r="52">
       <c r="A52">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
@@ -5787,7 +5787,7 @@
     </row>
     <row r="53">
       <c r="A53">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
@@ -5891,7 +5891,7 @@
     </row>
     <row r="54">
       <c r="A54">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
@@ -5995,7 +5995,7 @@
     </row>
     <row r="55">
       <c r="A55">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
@@ -6099,7 +6099,7 @@
     </row>
     <row r="56">
       <c r="A56">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
@@ -6203,7 +6203,7 @@
     </row>
     <row r="57">
       <c r="A57">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
@@ -6307,7 +6307,7 @@
     </row>
     <row r="58">
       <c r="A58">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
@@ -6411,7 +6411,7 @@
     </row>
     <row r="59">
       <c r="A59">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
@@ -6515,7 +6515,7 @@
     </row>
     <row r="60">
       <c r="A60">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
@@ -6619,7 +6619,7 @@
     </row>
     <row r="61">
       <c r="A61">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
@@ -6723,7 +6723,7 @@
     </row>
     <row r="62">
       <c r="A62">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
@@ -6827,7 +6827,7 @@
     </row>
     <row r="63">
       <c r="A63">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
@@ -6931,7 +6931,7 @@
     </row>
     <row r="64">
       <c r="A64">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
@@ -7035,7 +7035,7 @@
     </row>
     <row r="65">
       <c r="A65">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
@@ -7139,7 +7139,7 @@
     </row>
     <row r="66">
       <c r="A66">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
@@ -7243,7 +7243,7 @@
     </row>
     <row r="67">
       <c r="A67">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
@@ -7347,7 +7347,7 @@
     </row>
     <row r="68">
       <c r="A68">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
@@ -7451,7 +7451,7 @@
     </row>
     <row r="69">
       <c r="A69">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
@@ -7555,7 +7555,7 @@
     </row>
     <row r="70">
       <c r="A70">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
@@ -7659,7 +7659,7 @@
     </row>
     <row r="71">
       <c r="A71">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
@@ -7763,7 +7763,7 @@
     </row>
     <row r="72">
       <c r="A72">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
@@ -7867,7 +7867,7 @@
     </row>
     <row r="73">
       <c r="A73">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
@@ -7971,7 +7971,7 @@
     </row>
     <row r="74">
       <c r="A74">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
@@ -8075,7 +8075,7 @@
     </row>
     <row r="75">
       <c r="A75">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
@@ -8179,7 +8179,7 @@
     </row>
     <row r="76">
       <c r="A76">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
@@ -8283,7 +8283,7 @@
     </row>
     <row r="77">
       <c r="A77">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
@@ -8381,7 +8381,7 @@
     </row>
     <row r="78">
       <c r="A78">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
@@ -8479,7 +8479,7 @@
     </row>
     <row r="79">
       <c r="A79">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
@@ -8577,7 +8577,7 @@
     </row>
     <row r="80">
       <c r="A80">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
@@ -8675,7 +8675,7 @@
     </row>
     <row r="81">
       <c r="A81">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
@@ -8773,7 +8773,7 @@
     </row>
     <row r="82">
       <c r="A82">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
@@ -8871,7 +8871,7 @@
     </row>
     <row r="83">
       <c r="A83">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
@@ -8969,7 +8969,7 @@
     </row>
     <row r="84">
       <c r="A84">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
@@ -9067,7 +9067,7 @@
     </row>
     <row r="85">
       <c r="A85">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
@@ -9165,7 +9165,7 @@
     </row>
     <row r="86">
       <c r="A86">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
@@ -9263,7 +9263,7 @@
     </row>
     <row r="87">
       <c r="A87">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
@@ -9361,7 +9361,7 @@
     </row>
     <row r="88">
       <c r="A88">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
@@ -9459,7 +9459,7 @@
     </row>
     <row r="89">
       <c r="A89">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
@@ -9557,7 +9557,7 @@
     </row>
     <row r="90">
       <c r="A90">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
@@ -9655,7 +9655,7 @@
     </row>
     <row r="91">
       <c r="A91">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
@@ -9753,7 +9753,7 @@
     </row>
     <row r="92">
       <c r="A92">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
@@ -9851,7 +9851,7 @@
     </row>
     <row r="93">
       <c r="A93">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
@@ -9949,7 +9949,7 @@
     </row>
     <row r="94">
       <c r="A94">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
@@ -10047,7 +10047,7 @@
     </row>
     <row r="95">
       <c r="A95">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
@@ -10145,7 +10145,7 @@
     </row>
     <row r="96">
       <c r="A96">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
@@ -10243,7 +10243,7 @@
     </row>
     <row r="97">
       <c r="A97">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
@@ -10341,7 +10341,7 @@
     </row>
     <row r="98">
       <c r="A98">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
@@ -10439,7 +10439,7 @@
     </row>
     <row r="99">
       <c r="A99">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
@@ -10537,7 +10537,7 @@
     </row>
     <row r="100">
       <c r="A100">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
@@ -10635,7 +10635,7 @@
     </row>
     <row r="101">
       <c r="A101">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
@@ -10733,7 +10733,7 @@
     </row>
     <row r="102">
       <c r="A102">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
@@ -10831,7 +10831,7 @@
     </row>
     <row r="103">
       <c r="A103">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
@@ -10929,7 +10929,7 @@
     </row>
     <row r="104">
       <c r="A104">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
@@ -11027,7 +11027,7 @@
     </row>
     <row r="105">
       <c r="A105">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
@@ -11125,7 +11125,7 @@
     </row>
     <row r="106">
       <c r="A106">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
@@ -11223,7 +11223,7 @@
     </row>
     <row r="107">
       <c r="A107">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
@@ -11321,7 +11321,7 @@
     </row>
     <row r="108">
       <c r="A108">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
@@ -11419,7 +11419,7 @@
     </row>
     <row r="109">
       <c r="A109">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
@@ -11517,7 +11517,7 @@
     </row>
     <row r="110">
       <c r="A110">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
@@ -11615,7 +11615,7 @@
     </row>
     <row r="111">
       <c r="A111">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
@@ -11713,7 +11713,7 @@
     </row>
     <row r="112">
       <c r="A112">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
@@ -11811,7 +11811,7 @@
     </row>
     <row r="113">
       <c r="A113">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
@@ -11909,7 +11909,7 @@
     </row>
     <row r="114">
       <c r="A114">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
@@ -12007,7 +12007,7 @@
     </row>
     <row r="115">
       <c r="A115">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
@@ -12105,7 +12105,7 @@
     </row>
     <row r="116">
       <c r="A116">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
@@ -12203,7 +12203,7 @@
     </row>
     <row r="117">
       <c r="A117">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
@@ -12301,7 +12301,7 @@
     </row>
     <row r="118">
       <c r="A118">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
@@ -12399,7 +12399,7 @@
     </row>
     <row r="119">
       <c r="A119">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
@@ -12497,7 +12497,7 @@
     </row>
     <row r="120">
       <c r="A120">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
@@ -12595,7 +12595,7 @@
     </row>
     <row r="121">
       <c r="A121">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
@@ -12693,7 +12693,7 @@
     </row>
     <row r="122">
       <c r="A122">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
@@ -12791,7 +12791,7 @@
     </row>
     <row r="123">
       <c r="A123">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
@@ -12889,7 +12889,7 @@
     </row>
     <row r="124">
       <c r="A124">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
@@ -12987,7 +12987,7 @@
     </row>
     <row r="125">
       <c r="A125">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
@@ -13085,7 +13085,7 @@
     </row>
     <row r="126">
       <c r="A126">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
@@ -13183,7 +13183,7 @@
     </row>
     <row r="127">
       <c r="A127">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
@@ -13281,7 +13281,7 @@
     </row>
     <row r="128">
       <c r="A128">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="B128" t="inlineStr">
         <is>
@@ -13379,7 +13379,7 @@
     </row>
     <row r="129">
       <c r="A129">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="B129" t="inlineStr">
         <is>
@@ -13477,7 +13477,7 @@
     </row>
     <row r="130">
       <c r="A130">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="B130" t="inlineStr">
         <is>
@@ -13575,7 +13575,7 @@
     </row>
     <row r="131">
       <c r="A131">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="B131" t="inlineStr">
         <is>
@@ -13673,7 +13673,7 @@
     </row>
     <row r="132">
       <c r="A132">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="B132" t="inlineStr">
         <is>
@@ -13771,7 +13771,7 @@
     </row>
     <row r="133">
       <c r="A133">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="B133" t="inlineStr">
         <is>
@@ -13869,7 +13869,7 @@
     </row>
     <row r="134">
       <c r="A134">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="B134" t="inlineStr">
         <is>
@@ -13967,7 +13967,7 @@
     </row>
     <row r="135">
       <c r="A135">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="B135" t="inlineStr">
         <is>
@@ -14065,7 +14065,7 @@
     </row>
     <row r="136">
       <c r="A136">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="B136" t="inlineStr">
         <is>
@@ -14163,7 +14163,7 @@
     </row>
     <row r="137">
       <c r="A137">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="B137" t="inlineStr">
         <is>
@@ -14261,7 +14261,7 @@
     </row>
     <row r="138">
       <c r="A138">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="B138" t="inlineStr">
         <is>
@@ -14359,7 +14359,7 @@
     </row>
     <row r="139">
       <c r="A139">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="B139" t="inlineStr">
         <is>
@@ -14457,7 +14457,7 @@
     </row>
     <row r="140">
       <c r="A140">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="B140" t="inlineStr">
         <is>

</xml_diff>